<commit_message>
latest update from Narjes
</commit_message>
<xml_diff>
--- a/Resources/Database Diagram.xlsx
+++ b/Resources/Database Diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonof\UCSDProjects\Team-A-Kaggle_Brazilian_E_commerce\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Boot Camp\Homework\ETL project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5977F6A-B566-4C87-A30D-BD8ED4343F36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDD1CFF6-E1C1-43C0-9859-4DACD33F86E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6447C0C-CDE0-44DB-B773-F593A967F175}"/>
+    <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" activeTab="4" xr2:uid="{D6447C0C-CDE0-44DB-B773-F593A967F175}"/>
   </bookViews>
   <sheets>
     <sheet name="Data sets" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="171">
   <si>
     <t>customer_id</t>
   </si>
@@ -259,9 +259,6 @@
     <t>olist_orders_dataset (AMIR)</t>
   </si>
   <si>
-    <t>NVARCHAR(60)</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -524,6 +521,27 @@
   </si>
   <si>
     <t xml:space="preserve">CHANGED_BY </t>
+  </si>
+  <si>
+    <t>VarChar(50)</t>
+  </si>
+  <si>
+    <t>VarChar(40)</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>VarChar(15)</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -625,14 +643,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2809,44 +2827,44 @@
   <dimension ref="A3:H14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.42578125" customWidth="1"/>
-    <col min="5" max="5" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2854,20 +2872,20 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" t="str">
         <f>CONCATENATE("stg_",B4)</f>
         <v>stg_olist_customer_dataset</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2875,41 +2893,41 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ref="E5:E14" si="0">CONCATENATE("stg_",B5)</f>
         <v>stg_olist_geolocation_dataset</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_order_items_dataset</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2917,20 +2935,20 @@
         <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_order_payments_dataset</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2938,65 +2956,65 @@
         <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_order_reviews_dataset</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_orders_dataset</v>
       </c>
       <c r="G9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_products_dataset</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3004,86 +3022,86 @@
         <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_sellers_dataset</v>
       </c>
       <c r="F11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>stg_product_category_name_translation</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_marketing_qualified_leads_dataset</v>
       </c>
       <c r="G13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
         <v>92</v>
-      </c>
-      <c r="C14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" t="s">
-        <v>93</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>stg_olist_closed_deals_dataset</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3095,26 +3113,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD38FA21-38A4-4864-8FAF-3EEF1BAB0B21}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B21"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3139,10 +3157,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3153,7 +3171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3164,7 +3182,7 @@
         <v>14409</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3175,7 +3193,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3186,24 +3204,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -3218,7 +3236,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3229,10 +3247,10 @@
         <v>1037</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3243,10 +3261,10 @@
         <v>-23.545621281152599</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3257,10 +3275,10 @@
         <v>-46.6392920480016</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -3271,10 +3289,10 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -3285,49 +3303,49 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
-        <v>110</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="D21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="D23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -3341,7 +3359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3352,7 +3370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -3363,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3374,7 +3392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3385,7 +3403,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
@@ -3396,7 +3414,7 @@
         <v>42997.406655092593</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>6</v>
       </c>
@@ -3407,7 +3425,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -3418,14 +3436,14 @@
         <v>13.29</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
@@ -3439,7 +3457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -3449,8 +3467,11 @@
       <c r="C40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -3460,8 +3481,11 @@
       <c r="C41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -3471,8 +3495,11 @@
       <c r="C42" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4</v>
       </c>
@@ -3482,8 +3509,11 @@
       <c r="C43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5</v>
       </c>
@@ -3493,15 +3523,18 @@
       <c r="C44">
         <v>99.33</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+      <c r="D44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>11</v>
       </c>
@@ -3515,7 +3548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3525,8 +3558,11 @@
       <c r="C49" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -3536,8 +3572,11 @@
       <c r="C50" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>3</v>
       </c>
@@ -3547,24 +3586,33 @@
       <c r="C51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>4</v>
       </c>
       <c r="B52" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
       <c r="B53" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6</v>
       </c>
@@ -3574,8 +3622,11 @@
       <c r="C54" s="3">
         <v>43118</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>7</v>
       </c>
@@ -3585,15 +3636,18 @@
       <c r="C55" s="3">
         <v>43118.907627314817</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="D55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>11</v>
       </c>
@@ -3607,7 +3661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1</v>
       </c>
@@ -3617,8 +3671,11 @@
       <c r="C60" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2</v>
       </c>
@@ -3628,8 +3685,11 @@
       <c r="C61" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3</v>
       </c>
@@ -3640,10 +3700,10 @@
         <v>49</v>
       </c>
       <c r="D62" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4</v>
       </c>
@@ -3653,8 +3713,11 @@
       <c r="C63" s="3">
         <v>43010.455937500003</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>5</v>
       </c>
@@ -3664,8 +3727,11 @@
       <c r="C64" s="3">
         <v>43010.463368055556</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>6</v>
       </c>
@@ -3675,8 +3741,11 @@
       <c r="C65" s="3">
         <v>43012.829861111109</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>7</v>
       </c>
@@ -3686,8 +3755,11 @@
       <c r="C66" s="3">
         <v>43018.892511574071</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>8</v>
       </c>
@@ -3697,15 +3769,18 @@
       <c r="C67" s="3">
         <v>43026</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>11</v>
       </c>
@@ -3719,7 +3794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1</v>
       </c>
@@ -3730,7 +3805,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2</v>
       </c>
@@ -3741,7 +3816,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3</v>
       </c>
@@ -3752,10 +3827,10 @@
         <v>40</v>
       </c>
       <c r="D74" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4</v>
       </c>
@@ -3766,7 +3841,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>5</v>
       </c>
@@ -3777,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>6</v>
       </c>
@@ -3788,7 +3863,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>7</v>
       </c>
@@ -3799,7 +3874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>8</v>
       </c>
@@ -3810,7 +3885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>9</v>
       </c>
@@ -3821,14 +3896,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>11</v>
       </c>
@@ -3842,7 +3917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1</v>
       </c>
@@ -3853,7 +3928,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2</v>
       </c>
@@ -3864,7 +3939,7 @@
         <v>13023</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>3</v>
       </c>
@@ -3875,7 +3950,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -3886,15 +3961,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>11</v>
       </c>
@@ -3909,7 +3984,7 @@
       </c>
       <c r="H91" s="8"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1</v>
       </c>
@@ -3920,7 +3995,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2</v>
       </c>
@@ -3931,14 +4006,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B97" s="10"/>
-      <c r="C97" s="10"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>11</v>
       </c>
@@ -3952,58 +4027,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1</v>
       </c>
       <c r="B99" t="s">
+        <v>118</v>
+      </c>
+      <c r="C99" t="s">
         <v>119</v>
       </c>
-      <c r="C99" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C100" s="7">
         <v>43132</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>3</v>
       </c>
       <c r="B101" t="s">
+        <v>121</v>
+      </c>
+      <c r="C101" t="s">
         <v>122</v>
       </c>
-      <c r="C101" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>4</v>
       </c>
       <c r="B102" t="s">
+        <v>123</v>
+      </c>
+      <c r="C102" t="s">
         <v>124</v>
       </c>
-      <c r="C102" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>11</v>
       </c>
@@ -4017,18 +4092,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2</v>
       </c>
@@ -4036,124 +4111,124 @@
         <v>26</v>
       </c>
       <c r="C109" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>3</v>
       </c>
       <c r="B110" t="s">
+        <v>127</v>
+      </c>
+      <c r="C110" t="s">
         <v>128</v>
       </c>
-      <c r="C110" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>4</v>
       </c>
       <c r="B111" t="s">
+        <v>129</v>
+      </c>
+      <c r="C111" t="s">
         <v>130</v>
       </c>
-      <c r="C111" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>5</v>
       </c>
       <c r="B112" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C112" s="3">
         <v>43157.832569444443</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>6</v>
       </c>
       <c r="B113" t="s">
+        <v>132</v>
+      </c>
+      <c r="C113" t="s">
         <v>133</v>
       </c>
-      <c r="C113" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>7</v>
       </c>
       <c r="B114" t="s">
+        <v>134</v>
+      </c>
+      <c r="C114" t="s">
         <v>135</v>
       </c>
-      <c r="C114" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>8</v>
       </c>
       <c r="B115" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115" t="s">
         <v>137</v>
       </c>
-      <c r="C115" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>10</v>
       </c>
       <c r="B117" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>11</v>
       </c>
       <c r="B118" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>12</v>
       </c>
       <c r="B119" t="s">
+        <v>141</v>
+      </c>
+      <c r="C119" t="s">
         <v>142</v>
       </c>
-      <c r="C119" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>14</v>
       </c>
       <c r="B121" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -4161,17 +4236,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A90:C90"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="A106:C106"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A90:C90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4186,16 +4261,16 @@
       <selection activeCell="C4" sqref="C4:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
@@ -4209,7 +4284,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -4220,10 +4295,10 @@
         <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -4234,7 +4309,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -4245,10 +4320,10 @@
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -4259,7 +4334,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -4270,7 +4345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -4281,7 +4356,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -4292,7 +4367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -4303,7 +4378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -4314,43 +4389,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F13" s="7">
         <f ca="1">TODAY()</f>
         <v>44248</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>111</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
         <v>112</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>114</v>
-      </c>
-      <c r="F15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -4363,38 +4438,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3FFCCF-85ED-4059-9026-9FD119C11E9B}">
   <dimension ref="B1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:2" ht="33.6" x14ac:dyDescent="0.65">
       <c r="B1" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -4412,53 +4487,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D9DAD1-9CDE-4379-AD7B-C074435B0DB4}">
   <dimension ref="F1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F1" t="s">
+        <v>145</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
         <v>146</v>
       </c>
-      <c r="O1" s="5" t="s">
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K18" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="K5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="5" t="s">
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" t="s">
+    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" t="s">
+    <row r="22" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K23" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>